<commit_message>
Gráficos da página sócios
</commit_message>
<xml_diff>
--- a/html/socio/sistema/tabelas/pessoas_exemplo.xlsx
+++ b/html/socio/sistema/tabelas/pessoas_exemplo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichau\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F45648-926B-43E4-B754-E63A4C260B10}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF68A564-65F8-421C-BCBE-11A22888DC7C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4669,10 +4669,10 @@
     <t>28633-455</t>
   </si>
   <si>
+    <t>123.123.532-99</t>
+  </si>
+  <si>
     <t>029.648.317.69</t>
-  </si>
-  <si>
-    <t>064.139.410-14</t>
   </si>
 </sst>
 </file>
@@ -5023,8 +5023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="D153" sqref="D153"/>
+    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="E175" sqref="E175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10132,7 +10132,7 @@
         <v>1361</v>
       </c>
       <c r="B160" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="C160" t="s">
         <v>1362</v>
@@ -10836,7 +10836,7 @@
         <v>1544</v>
       </c>
       <c r="B182" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>1545</v>

</xml_diff>